<commit_message>
clean up intake import
</commit_message>
<xml_diff>
--- a/DECIS/Importing/Files/Donor Intake Sheet.xlsx
+++ b/DECIS/Importing/Files/Donor Intake Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mrah\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F4F704-EADD-47C4-A6E6-ED868B0A646B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE0A643-A10C-4E92-BB4D-D3A582CAEDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1155" yWindow="3315" windowWidth="21600" windowHeight="11385" xr2:uid="{06A39DA7-366E-4F96-817A-14AD30240AA6}"/>
   </bookViews>
@@ -100,7 +100,7 @@
     <t>fake@email.com</t>
   </si>
   <si>
-    <t>Intake test asset</t>
+    <t>Duplicate</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>